<commit_message>
Updates to Bull Trout ranks, minor changes
</commit_message>
<xml_diff>
--- a/Output/Bull_Trout_Habitat_Quality_PROTECTION_Methow_Entiat_Wenatchee_OKanogan.xlsx
+++ b/Output/Bull_Trout_Habitat_Quality_PROTECTION_Methow_Entiat_Wenatchee_OKanogan.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -477,83 +477,249 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>Twisp River Upper 02</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Methow</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Upper Twisp River</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+      <c r="I2">
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <v>5</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>5</v>
+      </c>
+      <c r="M2">
+        <v>5</v>
+      </c>
+      <c r="N2">
+        <v>5</v>
+      </c>
+      <c r="O2">
+        <v>3</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>5</v>
+      </c>
+      <c r="R2">
+        <v>3</v>
+      </c>
+      <c r="S2">
+        <v>5</v>
+      </c>
+      <c r="T2">
+        <v>37</v>
+      </c>
+      <c r="U2">
+        <v>0.8222222222222222</v>
+      </c>
+      <c r="V2">
+        <v>3</v>
+      </c>
+      <c r="W2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Twisp River Upper 03</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Methow</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Upper Twisp River</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="G3">
+        <v>5</v>
+      </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
+      <c r="I3">
+        <v>5</v>
+      </c>
+      <c r="J3">
+        <v>5</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>5</v>
+      </c>
+      <c r="M3">
+        <v>5</v>
+      </c>
+      <c r="N3">
+        <v>5</v>
+      </c>
+      <c r="O3">
+        <v>3</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>5</v>
+      </c>
+      <c r="R3">
+        <v>3</v>
+      </c>
+      <c r="S3">
+        <v>5</v>
+      </c>
+      <c r="T3">
+        <v>37</v>
+      </c>
+      <c r="U3">
+        <v>0.8222222222222222</v>
+      </c>
+      <c r="V3">
+        <v>3</v>
+      </c>
+      <c r="W3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
           <t>White River Lower 08</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>Wenatchee</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>Lower White River</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="G2">
-        <v>5</v>
-      </c>
-      <c r="H2">
-        <v>5</v>
-      </c>
-      <c r="I2">
-        <v>5</v>
-      </c>
-      <c r="J2">
-        <v>5</v>
-      </c>
-      <c r="K2">
-        <v>3</v>
-      </c>
-      <c r="L2">
-        <v>5</v>
-      </c>
-      <c r="M2">
-        <v>5</v>
-      </c>
-      <c r="N2">
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="J4">
+        <v>5</v>
+      </c>
+      <c r="K4">
+        <v>3</v>
+      </c>
+      <c r="L4">
+        <v>5</v>
+      </c>
+      <c r="M4">
+        <v>5</v>
+      </c>
+      <c r="N4">
         <v>1</v>
       </c>
-      <c r="O2">
+      <c r="O4">
         <v>1</v>
       </c>
-      <c r="P2">
-        <v>3</v>
-      </c>
-      <c r="Q2">
-        <v>5</v>
-      </c>
-      <c r="R2">
+      <c r="P4">
+        <v>3</v>
+      </c>
+      <c r="Q4">
+        <v>5</v>
+      </c>
+      <c r="R4">
         <v>4</v>
       </c>
-      <c r="S2">
-        <v>5</v>
-      </c>
-      <c r="T2">
+      <c r="S4">
+        <v>5</v>
+      </c>
+      <c r="T4">
         <v>34</v>
       </c>
-      <c r="U2">
+      <c r="U4">
         <v>0.7555555555555555</v>
       </c>
-      <c r="V2">
-        <v>5</v>
-      </c>
-      <c r="W2">
+      <c r="V4">
+        <v>5</v>
+      </c>
+      <c r="W4">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Push all the misc changes
Just did misc changes over the last couple months, wanted to push all the changes.
</commit_message>
<xml_diff>
--- a/Output/Bull_Trout_Habitat_Quality_PROTECTION_Methow_Entiat_Wenatchee_OKanogan.xlsx
+++ b/Output/Bull_Trout_Habitat_Quality_PROTECTION_Methow_Entiat_Wenatchee_OKanogan.xlsx
@@ -1522,7 +1522,7 @@
         <v>5</v>
       </c>
       <c r="N15" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="O15" t="n">
         <v>1</v>
@@ -1540,13 +1540,13 @@
         <v>5</v>
       </c>
       <c r="T15" t="n">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="U15" t="n">
-        <v>0.844444444444444</v>
+        <v>0.755555555555556</v>
       </c>
       <c r="V15" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="W15" t="n">
         <v>3</v>
@@ -1593,7 +1593,7 @@
         <v>5</v>
       </c>
       <c r="N16" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="O16" t="n">
         <v>5</v>
@@ -1611,16 +1611,16 @@
         <v>5</v>
       </c>
       <c r="T16" t="n">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="U16" t="n">
-        <v>0.888888888888889</v>
+        <v>0.977777777777778</v>
       </c>
       <c r="V16" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="W16" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Misc Updates, Updated Code for New Data
Include new remote sensing metrics and other new data that required updates to code.
</commit_message>
<xml_diff>
--- a/Output/Bull_Trout_Habitat_Quality_PROTECTION_Methow_Entiat_Wenatchee_OKanogan.xlsx
+++ b/Output/Bull_Trout_Habitat_Quality_PROTECTION_Methow_Entiat_Wenatchee_OKanogan.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t xml:space="preserve">ReachName</t>
   </si>
@@ -32,15 +32,6 @@
     <t xml:space="preserve">Bull.Trout.Reach</t>
   </si>
   <si>
-    <t xml:space="preserve">BankStability_score</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ChannelStability_score</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stability_Mean</t>
-  </si>
-  <si>
     <t xml:space="preserve">CoarseSubstrate_score</t>
   </si>
   <si>
@@ -101,12 +92,6 @@
     <t xml:space="preserve">Middle Chiwawa River</t>
   </si>
   <si>
-    <t xml:space="preserve">Chiwawa River Upper 02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Upper Chiwawa River</t>
-  </si>
-  <si>
     <t xml:space="preserve">Entiat River Lake 02</t>
   </si>
   <si>
@@ -131,9 +116,6 @@
     <t xml:space="preserve">Entiat River Lake 10</t>
   </si>
   <si>
-    <t xml:space="preserve">Entiat River Lake 11</t>
-  </si>
-  <si>
     <t xml:space="preserve">North Creek 01</t>
   </si>
   <si>
@@ -144,12 +126,6 @@
   </si>
   <si>
     <t xml:space="preserve">no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Panther Creek 01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Panther Creek</t>
   </si>
   <si>
     <t xml:space="preserve">Twisp River Headwaters 01</t>
@@ -578,34 +554,25 @@
       <c r="T1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G2" t="n">
         <v>5</v>
@@ -623,66 +590,57 @@
         <v>5</v>
       </c>
       <c r="L2" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M2" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N2" t="n">
         <v>5</v>
       </c>
       <c r="O2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P2" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Q2" t="n">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="R2" t="n">
-        <v>3</v>
+        <v>0.85</v>
       </c>
       <c r="S2" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="T2" t="n">
-        <v>39</v>
-      </c>
-      <c r="U2" t="n">
-        <v>0.866666666666667</v>
-      </c>
-      <c r="V2" t="n">
-        <v>3</v>
-      </c>
-      <c r="W2" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G3" t="n">
         <v>5</v>
       </c>
       <c r="H3" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I3" t="n">
         <v>5</v>
@@ -691,282 +649,246 @@
         <v>5</v>
       </c>
       <c r="K3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L3" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M3" t="n">
         <v>5</v>
       </c>
       <c r="N3" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O3" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="P3" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Q3" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="R3" t="n">
-        <v>4</v>
+        <v>0.75</v>
       </c>
       <c r="S3" t="n">
         <v>5</v>
       </c>
       <c r="T3" t="n">
-        <v>34</v>
-      </c>
-      <c r="U3" t="n">
-        <v>0.755555555555556</v>
-      </c>
-      <c r="V3" t="n">
-        <v>5</v>
-      </c>
-      <c r="W3" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G4" t="n">
         <v>5</v>
       </c>
       <c r="H4" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I4" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J4" t="n">
         <v>5</v>
       </c>
       <c r="K4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L4" t="n">
         <v>5</v>
       </c>
       <c r="M4" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N4" t="n">
         <v>5</v>
       </c>
       <c r="O4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="P4" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Q4" t="n">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="R4" t="n">
-        <v>4</v>
+        <v>0.775</v>
       </c>
       <c r="S4" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="T4" t="n">
-        <v>32</v>
-      </c>
-      <c r="U4" t="n">
-        <v>0.711111111111111</v>
-      </c>
-      <c r="V4" t="n">
-        <v>5</v>
-      </c>
-      <c r="W4" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" t="n">
+        <v>5</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" t="n">
+        <v>3</v>
+      </c>
+      <c r="J5" t="n">
+        <v>5</v>
+      </c>
+      <c r="K5" t="n">
+        <v>3</v>
+      </c>
+      <c r="L5" t="n">
+        <v>5</v>
+      </c>
+      <c r="M5" t="n">
+        <v>3</v>
+      </c>
+      <c r="N5" t="n">
+        <v>5</v>
+      </c>
+      <c r="O5" t="n">
+        <v>4</v>
+      </c>
+      <c r="P5" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q5" t="n">
         <v>31</v>
       </c>
-      <c r="B5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" t="n">
-        <v>3</v>
-      </c>
-      <c r="H5" t="n">
-        <v>5</v>
-      </c>
-      <c r="I5" t="n">
-        <v>4</v>
-      </c>
-      <c r="J5" t="n">
-        <v>5</v>
-      </c>
-      <c r="K5" t="n">
-        <v>1</v>
-      </c>
-      <c r="L5" t="n">
-        <v>3</v>
-      </c>
-      <c r="M5" t="n">
-        <v>5</v>
-      </c>
-      <c r="N5" t="n">
-        <v>3</v>
-      </c>
-      <c r="O5" t="n">
-        <v>5</v>
-      </c>
-      <c r="P5" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>5</v>
-      </c>
       <c r="R5" t="n">
-        <v>3</v>
+        <v>0.775</v>
       </c>
       <c r="S5" t="n">
         <v>5</v>
       </c>
       <c r="T5" t="n">
-        <v>34</v>
-      </c>
-      <c r="U5" t="n">
-        <v>0.755555555555556</v>
-      </c>
-      <c r="V5" t="n">
-        <v>5</v>
-      </c>
-      <c r="W5" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G6" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H6" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I6" t="n">
+        <v>3</v>
+      </c>
+      <c r="J6" t="n">
+        <v>5</v>
+      </c>
+      <c r="K6" t="n">
+        <v>3</v>
+      </c>
+      <c r="L6" t="n">
+        <v>5</v>
+      </c>
+      <c r="M6" t="n">
+        <v>3</v>
+      </c>
+      <c r="N6" t="n">
+        <v>5</v>
+      </c>
+      <c r="O6" t="n">
         <v>4</v>
       </c>
-      <c r="J6" t="n">
-        <v>5</v>
-      </c>
-      <c r="K6" t="n">
-        <v>1</v>
-      </c>
-      <c r="L6" t="n">
-        <v>3</v>
-      </c>
-      <c r="M6" t="n">
-        <v>5</v>
-      </c>
-      <c r="N6" t="n">
-        <v>3</v>
-      </c>
-      <c r="O6" t="n">
-        <v>5</v>
-      </c>
       <c r="P6" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Q6" t="n">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="R6" t="n">
-        <v>3</v>
+        <v>0.775</v>
       </c>
       <c r="S6" t="n">
         <v>5</v>
       </c>
       <c r="T6" t="n">
-        <v>34</v>
-      </c>
-      <c r="U6" t="n">
-        <v>0.755555555555556</v>
-      </c>
-      <c r="V6" t="n">
-        <v>5</v>
-      </c>
-      <c r="W6" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G7" t="n">
         <v>5</v>
       </c>
       <c r="H7" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I7" t="n">
         <v>5</v>
@@ -975,63 +897,54 @@
         <v>5</v>
       </c>
       <c r="K7" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L7" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M7" t="n">
         <v>5</v>
       </c>
       <c r="N7" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O7" t="n">
         <v>5</v>
       </c>
       <c r="P7" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Q7" t="n">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="R7" t="n">
-        <v>3</v>
+        <v>0.95</v>
       </c>
       <c r="S7" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="T7" t="n">
-        <v>35</v>
-      </c>
-      <c r="U7" t="n">
-        <v>0.777777777777778</v>
-      </c>
-      <c r="V7" t="n">
-        <v>5</v>
-      </c>
-      <c r="W7" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G8" t="n">
         <v>5</v>
@@ -1049,60 +962,51 @@
         <v>3</v>
       </c>
       <c r="L8" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M8" t="n">
         <v>5</v>
       </c>
       <c r="N8" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O8" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P8" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Q8" t="n">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="R8" t="n">
-        <v>4</v>
+        <v>0.875</v>
       </c>
       <c r="S8" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="T8" t="n">
-        <v>42</v>
-      </c>
-      <c r="U8" t="n">
-        <v>0.933333333333333</v>
-      </c>
-      <c r="V8" t="n">
-        <v>1</v>
-      </c>
-      <c r="W8" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G9" t="n">
         <v>5</v>
@@ -1117,10 +1021,10 @@
         <v>5</v>
       </c>
       <c r="K9" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L9" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M9" t="n">
         <v>5</v>
@@ -1129,51 +1033,42 @@
         <v>3</v>
       </c>
       <c r="O9" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P9" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Q9" t="n">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="R9" t="n">
-        <v>3</v>
+        <v>0.875</v>
       </c>
       <c r="S9" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="T9" t="n">
-        <v>39</v>
-      </c>
-      <c r="U9" t="n">
-        <v>0.866666666666667</v>
-      </c>
-      <c r="V9" t="n">
-        <v>3</v>
-      </c>
-      <c r="W9" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="F10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G10" t="n">
         <v>5</v>
@@ -1188,63 +1083,54 @@
         <v>5</v>
       </c>
       <c r="K10" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L10" t="n">
         <v>5</v>
       </c>
       <c r="M10" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N10" t="n">
         <v>3</v>
       </c>
       <c r="O10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P10" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Q10" t="n">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="R10" t="n">
-        <v>3</v>
+        <v>0.875</v>
       </c>
       <c r="S10" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="T10" t="n">
-        <v>39</v>
-      </c>
-      <c r="U10" t="n">
-        <v>0.866666666666667</v>
-      </c>
-      <c r="V10" t="n">
-        <v>3</v>
-      </c>
-      <c r="W10" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G11" t="n">
         <v>5</v>
@@ -1259,72 +1145,63 @@
         <v>5</v>
       </c>
       <c r="K11" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L11" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="M11" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N11" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O11" t="n">
         <v>3</v>
       </c>
       <c r="P11" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Q11" t="n">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="R11" t="n">
-        <v>4</v>
+        <v>0.95</v>
       </c>
       <c r="S11" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="T11" t="n">
-        <v>32</v>
-      </c>
-      <c r="U11" t="n">
-        <v>0.711111111111111</v>
-      </c>
-      <c r="V11" t="n">
-        <v>5</v>
-      </c>
-      <c r="W11" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" t="s">
         <v>40</v>
       </c>
-      <c r="B12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" t="s">
-        <v>42</v>
-      </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E12" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="F12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G12" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H12" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I12" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J12" t="n">
         <v>5</v>
@@ -1333,66 +1210,57 @@
         <v>5</v>
       </c>
       <c r="L12" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M12" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N12" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O12" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="P12" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Q12" t="n">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="R12" t="n">
-        <v>2</v>
+        <v>0.8</v>
       </c>
       <c r="S12" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="T12" t="n">
-        <v>39</v>
-      </c>
-      <c r="U12" t="n">
-        <v>0.866666666666667</v>
-      </c>
-      <c r="V12" t="n">
-        <v>3</v>
-      </c>
-      <c r="W12" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G13" t="n">
         <v>5</v>
       </c>
       <c r="H13" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I13" t="n">
         <v>5</v>
@@ -1401,69 +1269,60 @@
         <v>5</v>
       </c>
       <c r="K13" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L13" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M13" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N13" t="n">
         <v>5</v>
       </c>
       <c r="O13" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P13" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Q13" t="n">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="R13" t="n">
-        <v>4</v>
+        <v>0.8</v>
       </c>
       <c r="S13" t="n">
         <v>3</v>
       </c>
       <c r="T13" t="n">
-        <v>32</v>
-      </c>
-      <c r="U13" t="n">
-        <v>0.711111111111111</v>
-      </c>
-      <c r="V13" t="n">
-        <v>5</v>
-      </c>
-      <c r="W13" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G14" t="n">
         <v>5</v>
       </c>
       <c r="H14" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I14" t="n">
         <v>5</v>
@@ -1472,69 +1331,60 @@
         <v>5</v>
       </c>
       <c r="K14" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L14" t="n">
         <v>5</v>
       </c>
       <c r="M14" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N14" t="n">
         <v>5</v>
       </c>
       <c r="O14" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P14" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Q14" t="n">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="R14" t="n">
-        <v>3</v>
+        <v>0.825</v>
       </c>
       <c r="S14" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="T14" t="n">
-        <v>43</v>
-      </c>
-      <c r="U14" t="n">
-        <v>0.955555555555556</v>
-      </c>
-      <c r="V14" t="n">
-        <v>1</v>
-      </c>
-      <c r="W14" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E15" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F15" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G15" t="n">
         <v>5</v>
       </c>
       <c r="H15" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I15" t="n">
         <v>5</v>
@@ -1543,69 +1393,60 @@
         <v>5</v>
       </c>
       <c r="K15" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L15" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M15" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N15" t="n">
         <v>5</v>
       </c>
       <c r="O15" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P15" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Q15" t="n">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="R15" t="n">
-        <v>3</v>
+        <v>0.725</v>
       </c>
       <c r="S15" t="n">
         <v>5</v>
       </c>
       <c r="T15" t="n">
-        <v>37</v>
-      </c>
-      <c r="U15" t="n">
-        <v>0.822222222222222</v>
-      </c>
-      <c r="V15" t="n">
-        <v>3</v>
-      </c>
-      <c r="W15" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G16" t="n">
         <v>5</v>
       </c>
       <c r="H16" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I16" t="n">
         <v>5</v>
@@ -1614,69 +1455,60 @@
         <v>5</v>
       </c>
       <c r="K16" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L16" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M16" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N16" t="n">
         <v>5</v>
       </c>
       <c r="O16" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P16" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Q16" t="n">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="R16" t="n">
-        <v>3</v>
+        <v>0.775</v>
       </c>
       <c r="S16" t="n">
         <v>5</v>
       </c>
       <c r="T16" t="n">
-        <v>37</v>
-      </c>
-      <c r="U16" t="n">
-        <v>0.822222222222222</v>
-      </c>
-      <c r="V16" t="n">
-        <v>3</v>
-      </c>
-      <c r="W16" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G17" t="n">
         <v>5</v>
       </c>
       <c r="H17" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I17" t="n">
         <v>5</v>
@@ -1688,66 +1520,57 @@
         <v>1</v>
       </c>
       <c r="L17" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M17" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N17" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O17" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="P17" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Q17" t="n">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="R17" t="n">
-        <v>4</v>
+        <v>0.7</v>
       </c>
       <c r="S17" t="n">
         <v>5</v>
       </c>
       <c r="T17" t="n">
-        <v>38</v>
-      </c>
-      <c r="U17" t="n">
-        <v>0.844444444444444</v>
-      </c>
-      <c r="V17" t="n">
-        <v>3</v>
-      </c>
-      <c r="W17" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D18" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E18" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F18" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G18" t="n">
         <v>5</v>
       </c>
       <c r="H18" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I18" t="n">
         <v>5</v>
@@ -1756,69 +1579,60 @@
         <v>5</v>
       </c>
       <c r="K18" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L18" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M18" t="n">
         <v>5</v>
       </c>
       <c r="N18" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O18" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="P18" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q18" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="R18" t="n">
-        <v>3</v>
+        <v>0.75</v>
       </c>
       <c r="S18" t="n">
         <v>5</v>
       </c>
       <c r="T18" t="n">
-        <v>33</v>
-      </c>
-      <c r="U18" t="n">
-        <v>0.733333333333333</v>
-      </c>
-      <c r="V18" t="n">
-        <v>5</v>
-      </c>
-      <c r="W18" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D19" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E19" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F19" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G19" t="n">
         <v>5</v>
       </c>
       <c r="H19" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I19" t="n">
         <v>5</v>
@@ -1833,249 +1647,27 @@
         <v>5</v>
       </c>
       <c r="M19" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N19" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O19" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P19" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Q19" t="n">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="R19" t="n">
-        <v>3</v>
+        <v>0.8</v>
       </c>
       <c r="S19" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="T19" t="n">
-        <v>35</v>
-      </c>
-      <c r="U19" t="n">
-        <v>0.777777777777778</v>
-      </c>
-      <c r="V19" t="n">
-        <v>5</v>
-      </c>
-      <c r="W19" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>54</v>
-      </c>
-      <c r="B20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" t="s">
-        <v>52</v>
-      </c>
-      <c r="D20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E20" t="s">
-        <v>26</v>
-      </c>
-      <c r="F20" t="s">
-        <v>26</v>
-      </c>
-      <c r="G20" t="n">
-        <v>5</v>
-      </c>
-      <c r="H20" t="n">
-        <v>5</v>
-      </c>
-      <c r="I20" t="n">
-        <v>5</v>
-      </c>
-      <c r="J20" t="n">
-        <v>5</v>
-      </c>
-      <c r="K20" t="n">
-        <v>3</v>
-      </c>
-      <c r="L20" t="n">
-        <v>5</v>
-      </c>
-      <c r="M20" t="n">
-        <v>5</v>
-      </c>
-      <c r="N20" t="n">
-        <v>1</v>
-      </c>
-      <c r="O20" t="n">
-        <v>1</v>
-      </c>
-      <c r="P20" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q20" t="n">
-        <v>5</v>
-      </c>
-      <c r="R20" t="n">
-        <v>3</v>
-      </c>
-      <c r="S20" t="n">
-        <v>5</v>
-      </c>
-      <c r="T20" t="n">
-        <v>33</v>
-      </c>
-      <c r="U20" t="n">
-        <v>0.733333333333333</v>
-      </c>
-      <c r="V20" t="n">
-        <v>5</v>
-      </c>
-      <c r="W20" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>55</v>
-      </c>
-      <c r="B21" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" t="s">
-        <v>52</v>
-      </c>
-      <c r="D21" t="s">
-        <v>26</v>
-      </c>
-      <c r="E21" t="s">
-        <v>26</v>
-      </c>
-      <c r="F21" t="s">
-        <v>26</v>
-      </c>
-      <c r="G21" t="n">
-        <v>5</v>
-      </c>
-      <c r="H21" t="n">
-        <v>5</v>
-      </c>
-      <c r="I21" t="n">
-        <v>5</v>
-      </c>
-      <c r="J21" t="n">
-        <v>5</v>
-      </c>
-      <c r="K21" t="n">
-        <v>1</v>
-      </c>
-      <c r="L21" t="n">
-        <v>5</v>
-      </c>
-      <c r="M21" t="n">
-        <v>5</v>
-      </c>
-      <c r="N21" t="n">
-        <v>5</v>
-      </c>
-      <c r="O21" t="n">
-        <v>1</v>
-      </c>
-      <c r="P21" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q21" t="n">
-        <v>5</v>
-      </c>
-      <c r="R21" t="n">
-        <v>3</v>
-      </c>
-      <c r="S21" t="n">
-        <v>3</v>
-      </c>
-      <c r="T21" t="n">
-        <v>33</v>
-      </c>
-      <c r="U21" t="n">
-        <v>0.733333333333333</v>
-      </c>
-      <c r="V21" t="n">
-        <v>5</v>
-      </c>
-      <c r="W21" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>56</v>
-      </c>
-      <c r="B22" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" t="s">
-        <v>57</v>
-      </c>
-      <c r="D22" t="s">
-        <v>26</v>
-      </c>
-      <c r="E22" t="s">
-        <v>26</v>
-      </c>
-      <c r="F22" t="s">
-        <v>26</v>
-      </c>
-      <c r="G22" t="n">
-        <v>5</v>
-      </c>
-      <c r="H22" t="n">
-        <v>5</v>
-      </c>
-      <c r="I22" t="n">
-        <v>5</v>
-      </c>
-      <c r="J22" t="n">
-        <v>5</v>
-      </c>
-      <c r="K22" t="n">
-        <v>3</v>
-      </c>
-      <c r="L22" t="n">
-        <v>5</v>
-      </c>
-      <c r="M22" t="n">
-        <v>5</v>
-      </c>
-      <c r="N22" t="n">
-        <v>1</v>
-      </c>
-      <c r="O22" t="n">
-        <v>5</v>
-      </c>
-      <c r="P22" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q22" t="n">
-        <v>3</v>
-      </c>
-      <c r="R22" t="n">
-        <v>3</v>
-      </c>
-      <c r="S22" t="n">
-        <v>5</v>
-      </c>
-      <c r="T22" t="n">
-        <v>37</v>
-      </c>
-      <c r="U22" t="n">
-        <v>0.822222222222222</v>
-      </c>
-      <c r="V22" t="n">
-        <v>3</v>
-      </c>
-      <c r="W22" t="n">
         <v>3</v>
       </c>
     </row>

</xml_diff>